<commit_message>
Revised Scripts 7 and 8
Scripts 7-* were unified in 7-Exposure (with additional comments and formulae); also, to produce the outputs of those scripts, ADH codes needed to be added.
Script 8 was revised too.
</commit_message>
<xml_diff>
--- a/1-Data-Codes/2-Final_Data/exposures.xlsx
+++ b/1-Data-Codes/2-Final_Data/exposures.xlsx
@@ -391,16 +391,16 @@
         </is>
       </c>
       <c r="B2">
-        <v>0.01740469228706648</v>
+        <v>0.01616742878187598</v>
       </c>
       <c r="C2">
-        <v>0.01654041841571729</v>
+        <v>0.01535950246713094</v>
       </c>
       <c r="D2">
-        <v>0.0104079778198634</v>
+        <v>0.01040797675305219</v>
       </c>
       <c r="E2">
-        <v>0.009853175537074745</v>
+        <v>0.009853174483103831</v>
       </c>
     </row>
     <row r="3">
@@ -410,16 +410,16 @@
         </is>
       </c>
       <c r="B3">
-        <v>0.001064138061892813</v>
+        <v>0.001114328573829887</v>
       </c>
       <c r="C3">
-        <v>0.0008082525302238881</v>
+        <v>0.0008352419201105366</v>
       </c>
       <c r="D3">
-        <v>0.000640974294239542</v>
+        <v>0.00064097576404339</v>
       </c>
       <c r="E3">
-        <v>0.0004244143757820513</v>
+        <v>0.000424415880559696</v>
       </c>
     </row>
     <row r="4">
@@ -429,16 +429,16 @@
         </is>
       </c>
       <c r="B4">
-        <v>0.008852108084066378</v>
+        <v>0.009290194329385984</v>
       </c>
       <c r="C4">
-        <v>0.008503132250578386</v>
+        <v>0.008958292485214825</v>
       </c>
       <c r="D4">
-        <v>0.004893050789723919</v>
+        <v>0.004893051700205482</v>
       </c>
       <c r="E4">
-        <v>0.004628879292681787</v>
+        <v>0.004628880236844239</v>
       </c>
     </row>
     <row r="5">
@@ -448,16 +448,16 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.01162382832018562</v>
+        <v>0.01082461737011016</v>
       </c>
       <c r="C5">
-        <v>0.01079910249285567</v>
+        <v>0.01005121773483124</v>
       </c>
       <c r="D5">
-        <v>0.007844856435932527</v>
+        <v>0.007844856199036571</v>
       </c>
       <c r="E5">
-        <v>0.007249515104500511</v>
+        <v>0.007249514974529432</v>
       </c>
     </row>
     <row r="6">
@@ -467,16 +467,16 @@
         </is>
       </c>
       <c r="B6">
-        <v>0.01310785847144861</v>
+        <v>0.01319984283752404</v>
       </c>
       <c r="C6">
-        <v>0.01267771675281943</v>
+        <v>0.01277067466336601</v>
       </c>
       <c r="D6">
-        <v>0.00711232916864492</v>
+        <v>0.007112328793891514</v>
       </c>
       <c r="E6">
-        <v>0.006722986841295486</v>
+        <v>0.006722986527750268</v>
       </c>
     </row>
     <row r="7">
@@ -486,16 +486,16 @@
         </is>
       </c>
       <c r="B7">
-        <v>0.007996963228433684</v>
+        <v>0.008543329123849633</v>
       </c>
       <c r="C7">
-        <v>0.007657236514422938</v>
+        <v>0.008199587688978913</v>
       </c>
       <c r="D7">
-        <v>0.003724351884581838</v>
+        <v>0.003724351013207759</v>
       </c>
       <c r="E7">
-        <v>0.00339323930168769</v>
+        <v>0.003393238323957433</v>
       </c>
     </row>
     <row r="8">
@@ -505,16 +505,16 @@
         </is>
       </c>
       <c r="B8">
-        <v>0.01033656794316028</v>
+        <v>0.01046547667246475</v>
       </c>
       <c r="C8">
-        <v>0.009848681964819238</v>
+        <v>0.009978790217379128</v>
       </c>
       <c r="D8">
-        <v>0.006377562480451919</v>
+        <v>0.006377560521764486</v>
       </c>
       <c r="E8">
-        <v>0.005970870924020959</v>
+        <v>0.005970869004540304</v>
       </c>
     </row>
     <row r="9">
@@ -524,16 +524,16 @@
         </is>
       </c>
       <c r="B9">
-        <v>0.00655438950285437</v>
+        <v>0.006746097520709175</v>
       </c>
       <c r="C9">
-        <v>0.005986586714858713</v>
+        <v>0.006172798679333302</v>
       </c>
       <c r="D9">
-        <v>0.003954658219529825</v>
+        <v>0.003954659092644731</v>
       </c>
       <c r="E9">
-        <v>0.003557966879887878</v>
+        <v>0.003557967823791874</v>
       </c>
     </row>
     <row r="10">
@@ -543,16 +543,16 @@
         </is>
       </c>
       <c r="B10">
-        <v>0.005495316962924581</v>
+        <v>0.005483029921715594</v>
       </c>
       <c r="C10">
-        <v>0.005165233135324227</v>
+        <v>0.005155526931975511</v>
       </c>
       <c r="D10">
-        <v>0.003090601138019741</v>
+        <v>0.003090602083261646</v>
       </c>
       <c r="E10">
-        <v>0.002874829040100625</v>
+        <v>0.002874829909109175</v>
       </c>
     </row>
     <row r="11">
@@ -562,16 +562,16 @@
         </is>
       </c>
       <c r="B11">
-        <v>0.0154670886458444</v>
+        <v>0.01448594085095975</v>
       </c>
       <c r="C11">
-        <v>0.01478210564764892</v>
+        <v>0.01384006079669633</v>
       </c>
       <c r="D11">
-        <v>0.009090665985282796</v>
+        <v>0.009090666601977554</v>
       </c>
       <c r="E11">
-        <v>0.008630940384025482</v>
+        <v>0.008630940929512132</v>
       </c>
     </row>
     <row r="12">
@@ -581,16 +581,16 @@
         </is>
       </c>
       <c r="B12">
-        <v>0.001847830307249824</v>
+        <v>0.002000943134382114</v>
       </c>
       <c r="C12">
-        <v>0.001682566464049795</v>
+        <v>0.00183203518568754</v>
       </c>
       <c r="D12">
-        <v>0.001250259928587364</v>
+        <v>0.001250260188395416</v>
       </c>
       <c r="E12">
-        <v>0.001141551703426879</v>
+        <v>0.001141551960656306</v>
       </c>
     </row>
     <row r="13">
@@ -600,16 +600,16 @@
         </is>
       </c>
       <c r="B13">
-        <v>0.009199343067260305</v>
+        <v>0.01091110483096589</v>
       </c>
       <c r="C13">
-        <v>0.008800877749656315</v>
+        <v>0.01054835723117971</v>
       </c>
       <c r="D13">
-        <v>0.005443221223128375</v>
+        <v>0.00544322307014899</v>
       </c>
       <c r="E13">
-        <v>0.005163415377313476</v>
+        <v>0.005163417245089633</v>
       </c>
     </row>
     <row r="14">
@@ -619,16 +619,16 @@
         </is>
       </c>
       <c r="B14">
-        <v>0.01076903227993569</v>
+        <v>0.01076224225654533</v>
       </c>
       <c r="C14">
-        <v>0.01013568676445963</v>
+        <v>0.01016446463892172</v>
       </c>
       <c r="D14">
-        <v>0.00670298478078545</v>
+        <v>0.006702984189505901</v>
       </c>
       <c r="E14">
-        <v>0.0062786005022627</v>
+        <v>0.006278599911020546</v>
       </c>
     </row>
     <row r="15">
@@ -638,16 +638,16 @@
         </is>
       </c>
       <c r="B15">
-        <v>0.01277846220815437</v>
+        <v>0.01211972355305121</v>
       </c>
       <c r="C15">
-        <v>0.01179083810006734</v>
+        <v>0.01120085889924361</v>
       </c>
       <c r="D15">
-        <v>0.008425643886056558</v>
+        <v>0.00842564417297337</v>
       </c>
       <c r="E15">
-        <v>0.007754813125508958</v>
+        <v>0.007754813363969747</v>
       </c>
     </row>
     <row r="16">
@@ -657,16 +657,16 @@
         </is>
       </c>
       <c r="B16">
-        <v>0.01176830802169334</v>
+        <v>0.01136176617822109</v>
       </c>
       <c r="C16">
-        <v>0.01107051633922004</v>
+        <v>0.01071036825864781</v>
       </c>
       <c r="D16">
-        <v>0.005820276602006415</v>
+        <v>0.005820276668568027</v>
       </c>
       <c r="E16">
-        <v>0.005394835714898369</v>
+        <v>0.005394835762708667</v>
       </c>
     </row>
     <row r="17">
@@ -676,16 +676,16 @@
         </is>
       </c>
       <c r="B17">
-        <v>0.006642182627982347</v>
+        <v>0.006688846828023988</v>
       </c>
       <c r="C17">
-        <v>0.005990610232911844</v>
+        <v>0.006054300513150836</v>
       </c>
       <c r="D17">
-        <v>0.004180088908538012</v>
+        <v>0.004180089349575281</v>
       </c>
       <c r="E17">
-        <v>0.003742261673949242</v>
+        <v>0.003742262109886662</v>
       </c>
     </row>
     <row r="18">
@@ -695,16 +695,16 @@
         </is>
       </c>
       <c r="B18">
-        <v>0.01139375262319232</v>
+        <v>0.01129602691239412</v>
       </c>
       <c r="C18">
-        <v>0.01062422407590595</v>
+        <v>0.01052716486314972</v>
       </c>
       <c r="D18">
-        <v>0.00744910647825863</v>
+        <v>0.007449106164755814</v>
       </c>
       <c r="E18">
-        <v>0.006928756595371975</v>
+        <v>0.006928756260441483</v>
       </c>
     </row>
     <row r="19">
@@ -714,16 +714,16 @@
         </is>
       </c>
       <c r="B19">
-        <v>0.004652091949659549</v>
+        <v>0.004499584297299004</v>
       </c>
       <c r="C19">
-        <v>0.004074712925308045</v>
+        <v>0.003941025107596979</v>
       </c>
       <c r="D19">
-        <v>0.002718475723688833</v>
+        <v>0.002718475176371824</v>
       </c>
       <c r="E19">
-        <v>0.002374592097611275</v>
+        <v>0.00237459151095364</v>
       </c>
     </row>
     <row r="20">
@@ -733,16 +733,16 @@
         </is>
       </c>
       <c r="B20">
-        <v>0.01101265882153492</v>
+        <v>0.01084744266142097</v>
       </c>
       <c r="C20">
-        <v>0.01043836616177143</v>
+        <v>0.01030271913191642</v>
       </c>
       <c r="D20">
-        <v>0.006697436111134449</v>
+        <v>0.006697436175344562</v>
       </c>
       <c r="E20">
-        <v>0.006314777904538574</v>
+        <v>0.006314777907923325</v>
       </c>
     </row>
     <row r="21">
@@ -752,16 +752,16 @@
         </is>
       </c>
       <c r="B21">
-        <v>0.005720049786656577</v>
+        <v>0.005576508910145192</v>
       </c>
       <c r="C21">
-        <v>0.005426612069355078</v>
+        <v>0.005295299990651683</v>
       </c>
       <c r="D21">
-        <v>0.002801671137003139</v>
+        <v>0.002801671083293092</v>
       </c>
       <c r="E21">
-        <v>0.002578702218209118</v>
+        <v>0.002578702215205706</v>
       </c>
     </row>
     <row r="22">
@@ -771,16 +771,16 @@
         </is>
       </c>
       <c r="B22">
-        <v>0.01315924226910122</v>
+        <v>0.01325244862305611</v>
       </c>
       <c r="C22">
-        <v>0.01272897061110784</v>
+        <v>0.01284031242119282</v>
       </c>
       <c r="D22">
-        <v>0.007132278760640352</v>
+        <v>0.00713227731343879</v>
       </c>
       <c r="E22">
-        <v>0.006721392517498132</v>
+        <v>0.006721391072394573</v>
       </c>
     </row>
     <row r="23">
@@ -790,16 +790,16 @@
         </is>
       </c>
       <c r="B23">
-        <v>0.009301068056193879</v>
+        <v>0.009144640966304907</v>
       </c>
       <c r="C23">
-        <v>0.00845082879195899</v>
+        <v>0.008311652321969835</v>
       </c>
       <c r="D23">
-        <v>0.0071635853646961</v>
+        <v>0.007163586037232712</v>
       </c>
       <c r="E23">
-        <v>0.00655680140505789</v>
+        <v>0.006556802097237505</v>
       </c>
     </row>
     <row r="24">
@@ -809,16 +809,16 @@
         </is>
       </c>
       <c r="B24">
-        <v>0.01092093823701655</v>
+        <v>0.01119555474451042</v>
       </c>
       <c r="C24">
-        <v>0.01025866467831402</v>
+        <v>0.01056478702123411</v>
       </c>
       <c r="D24">
-        <v>0.006256188773145984</v>
+        <v>0.006256189675348401</v>
       </c>
       <c r="E24">
-        <v>0.005750121617254366</v>
+        <v>0.005750122387365282</v>
       </c>
     </row>
     <row r="25">
@@ -828,16 +828,16 @@
         </is>
       </c>
       <c r="B25">
-        <v>0.01413927579208906</v>
+        <v>0.0126824240012623</v>
       </c>
       <c r="C25">
-        <v>0.01312666093257295</v>
+        <v>0.01176528219418757</v>
       </c>
       <c r="D25">
-        <v>0.009116557617433038</v>
+        <v>0.009116557752357634</v>
       </c>
       <c r="E25">
-        <v>0.008473568829274606</v>
+        <v>0.00847356898247313</v>
       </c>
     </row>
     <row r="26">
@@ -847,16 +847,16 @@
         </is>
       </c>
       <c r="B26">
-        <v>0.009815293322239025</v>
+        <v>0.009095738901378608</v>
       </c>
       <c r="C26">
-        <v>0.009154219549078028</v>
+        <v>0.008479899085518381</v>
       </c>
       <c r="D26">
-        <v>0.005403755124678399</v>
+        <v>0.005403753804922695</v>
       </c>
       <c r="E26">
-        <v>0.005002716608703664</v>
+        <v>0.00500271534161686</v>
       </c>
     </row>
     <row r="27">
@@ -866,16 +866,16 @@
         </is>
       </c>
       <c r="B27">
-        <v>0.002692378212257925</v>
+        <v>0.002886496802688513</v>
       </c>
       <c r="C27">
-        <v>0.002344968518395081</v>
+        <v>0.002551242442908614</v>
       </c>
       <c r="D27">
-        <v>0.001546523332050141</v>
+        <v>0.001546523188141996</v>
       </c>
       <c r="E27">
-        <v>0.001295201620571976</v>
+        <v>0.001295201366054413</v>
       </c>
     </row>
     <row r="28">
@@ -885,16 +885,16 @@
         </is>
       </c>
       <c r="B28">
-        <v>0.007476652159740717</v>
+        <v>0.007688735113494544</v>
       </c>
       <c r="C28">
-        <v>0.00696143175111672</v>
+        <v>0.007178040746313545</v>
       </c>
       <c r="D28">
-        <v>0.004541878414570482</v>
+        <v>0.004541879024141163</v>
       </c>
       <c r="E28">
-        <v>0.004196646120929682</v>
+        <v>0.004196646642253581</v>
       </c>
     </row>
     <row r="29">
@@ -904,16 +904,16 @@
         </is>
       </c>
       <c r="B29">
-        <v>0.00306080675124773</v>
+        <v>0.003102805861250911</v>
       </c>
       <c r="C29">
-        <v>0.002722908264783516</v>
+        <v>0.002783625130653979</v>
       </c>
       <c r="D29">
-        <v>0.001671506636993457</v>
+        <v>0.001671506828818534</v>
       </c>
       <c r="E29">
-        <v>0.001436346520318615</v>
+        <v>0.001436346759970835</v>
       </c>
     </row>
     <row r="30">
@@ -923,16 +923,16 @@
         </is>
       </c>
       <c r="B30">
-        <v>0.01690982566731769</v>
+        <v>0.01881836802423357</v>
       </c>
       <c r="C30">
-        <v>0.01635913006396045</v>
+        <v>0.01831705023945007</v>
       </c>
       <c r="D30">
-        <v>0.01008627706100606</v>
+        <v>0.01008627771016791</v>
       </c>
       <c r="E30">
-        <v>0.009601279122900234</v>
+        <v>0.009601279801896215</v>
       </c>
     </row>
     <row r="31">
@@ -942,16 +942,16 @@
         </is>
       </c>
       <c r="B31">
-        <v>0.009468426512062028</v>
+        <v>0.009520582340971785</v>
       </c>
       <c r="C31">
-        <v>0.008960878809554353</v>
+        <v>0.009021481541213466</v>
       </c>
       <c r="D31">
-        <v>0.005017335035629103</v>
+        <v>0.005017335486240285</v>
       </c>
       <c r="E31">
-        <v>0.004618584495904896</v>
+        <v>0.004618584966166936</v>
       </c>
     </row>
     <row r="32">
@@ -961,16 +961,16 @@
         </is>
       </c>
       <c r="B32">
-        <v>0.005270645194737419</v>
+        <v>0.005710218460705146</v>
       </c>
       <c r="C32">
-        <v>0.004906702433299748</v>
+        <v>0.005363264944307802</v>
       </c>
       <c r="D32">
-        <v>0.003088792425014819</v>
+        <v>0.003088792580914898</v>
       </c>
       <c r="E32">
-        <v>0.002813255801954871</v>
+        <v>0.002813255960366202</v>
       </c>
     </row>
     <row r="33">
@@ -980,16 +980,16 @@
         </is>
       </c>
       <c r="B33">
-        <v>0.009263276794848813</v>
+        <v>0.009059947259411177</v>
       </c>
       <c r="C33">
-        <v>0.008796666386126832</v>
+        <v>0.008633744800545042</v>
       </c>
       <c r="D33">
-        <v>0.005452606196576288</v>
+        <v>0.005452604803692462</v>
       </c>
       <c r="E33">
-        <v>0.005108976436053196</v>
+        <v>0.005108975033200711</v>
       </c>
     </row>
     <row r="34">
@@ -999,16 +999,16 @@
         </is>
       </c>
       <c r="B34">
-        <v>0.02216435593903707</v>
+        <v>0.02147791671006524</v>
       </c>
       <c r="C34">
-        <v>0.0211965646130035</v>
+        <v>0.02053408070452858</v>
       </c>
       <c r="D34">
-        <v>0.01383363544905441</v>
+        <v>0.01383363520534461</v>
       </c>
       <c r="E34">
-        <v>0.01316135730348048</v>
+        <v>0.0131613571126153</v>
       </c>
     </row>
     <row r="35">
@@ -1018,16 +1018,16 @@
         </is>
       </c>
       <c r="B35">
-        <v>0.003990259541291109</v>
+        <v>0.004288885526765049</v>
       </c>
       <c r="C35">
-        <v>0.003629687059670373</v>
+        <v>0.003923283735257924</v>
       </c>
       <c r="D35">
-        <v>0.002309732946265354</v>
+        <v>0.002309732435280013</v>
       </c>
       <c r="E35">
-        <v>0.002067386111202996</v>
+        <v>0.002067385597544581</v>
       </c>
     </row>
     <row r="36">
@@ -1037,16 +1037,16 @@
         </is>
       </c>
       <c r="B36">
-        <v>0.01158216091667626</v>
+        <v>0.01121122143878064</v>
       </c>
       <c r="C36">
-        <v>0.01066680234055277</v>
+        <v>0.01034648976974103</v>
       </c>
       <c r="D36">
-        <v>0.00724697138305599</v>
+        <v>0.007246972246919058</v>
       </c>
       <c r="E36">
-        <v>0.006655491154091646</v>
+        <v>0.006655491978484407</v>
       </c>
     </row>
     <row r="37">
@@ -1056,16 +1056,16 @@
         </is>
       </c>
       <c r="B37">
-        <v>0.008123718473361121</v>
+        <v>0.007799390664922923</v>
       </c>
       <c r="C37">
-        <v>0.007430775916479229</v>
+        <v>0.007153638715240352</v>
       </c>
       <c r="D37">
-        <v>0.004534899504586421</v>
+        <v>0.00453489937991951</v>
       </c>
       <c r="E37">
-        <v>0.004082787612524721</v>
+        <v>0.004082787516018557</v>
       </c>
     </row>
     <row r="38">
@@ -1075,16 +1075,16 @@
         </is>
       </c>
       <c r="B38">
-        <v>0.010569375823475</v>
+        <v>0.0113117412255217</v>
       </c>
       <c r="C38">
-        <v>0.01012769542607299</v>
+        <v>0.0108809700301654</v>
       </c>
       <c r="D38">
-        <v>0.006109762857778367</v>
+        <v>0.00610976309272813</v>
       </c>
       <c r="E38">
-        <v>0.005747578432740374</v>
+        <v>0.005747578644858038</v>
       </c>
     </row>
     <row r="39">
@@ -1094,16 +1094,16 @@
         </is>
       </c>
       <c r="B39">
-        <v>0.01214691883466969</v>
+        <v>0.01145575416434506</v>
       </c>
       <c r="C39">
-        <v>0.01136663061839803</v>
+        <v>0.01074719872271248</v>
       </c>
       <c r="D39">
-        <v>0.007340467944595148</v>
+        <v>0.007340469606039235</v>
       </c>
       <c r="E39">
-        <v>0.006833545102303642</v>
+        <v>0.006833546719119132</v>
       </c>
     </row>
     <row r="40">
@@ -1113,16 +1113,16 @@
         </is>
       </c>
       <c r="B40">
-        <v>0.01501295460503677</v>
+        <v>0.0150075520340855</v>
       </c>
       <c r="C40">
-        <v>0.01423001103437265</v>
+        <v>0.01421536947059665</v>
       </c>
       <c r="D40">
-        <v>0.00831953516904162</v>
+        <v>0.008319534145116261</v>
       </c>
       <c r="E40">
-        <v>0.007716745967718373</v>
+        <v>0.007716745000185323</v>
       </c>
     </row>
     <row r="41">
@@ -1132,16 +1132,16 @@
         </is>
       </c>
       <c r="B41">
-        <v>0.02186737697738163</v>
+        <v>0.02068201334671391</v>
       </c>
       <c r="C41">
-        <v>0.02095774614015163</v>
+        <v>0.0198143654646785</v>
       </c>
       <c r="D41">
-        <v>0.01333165117473448</v>
+        <v>0.01333165186640678</v>
       </c>
       <c r="E41">
-        <v>0.01275811575018004</v>
+        <v>0.01275811645578467</v>
       </c>
     </row>
     <row r="42">
@@ -1151,16 +1151,16 @@
         </is>
       </c>
       <c r="B42">
-        <v>0.007533601744883825</v>
+        <v>0.008408932922103374</v>
       </c>
       <c r="C42">
-        <v>0.00706876237914545</v>
+        <v>0.007914856691945908</v>
       </c>
       <c r="D42">
-        <v>0.00511870936894376</v>
+        <v>0.005118709533145206</v>
       </c>
       <c r="E42">
-        <v>0.004742293716065738</v>
+        <v>0.004742293969250113</v>
       </c>
     </row>
     <row r="43">
@@ -1170,16 +1170,16 @@
         </is>
       </c>
       <c r="B43">
-        <v>0.01451043534403034</v>
+        <v>0.01349271310064208</v>
       </c>
       <c r="C43">
-        <v>0.01363491576123426</v>
+        <v>0.01266955291028146</v>
       </c>
       <c r="D43">
-        <v>0.008366785394538253</v>
+        <v>0.008366784789245758</v>
       </c>
       <c r="E43">
-        <v>0.007805428799881726</v>
+        <v>0.007805428207260065</v>
       </c>
     </row>
     <row r="44">
@@ -1189,16 +1189,16 @@
         </is>
       </c>
       <c r="B44">
-        <v>0.009210328532476131</v>
+        <v>0.009571082311229008</v>
       </c>
       <c r="C44">
-        <v>0.008688224193069301</v>
+        <v>0.009073167220271241</v>
       </c>
       <c r="D44">
-        <v>0.005161834184881375</v>
+        <v>0.005161834156403239</v>
       </c>
       <c r="E44">
-        <v>0.004775816923017246</v>
+        <v>0.004775816941044946</v>
       </c>
     </row>
     <row r="45">
@@ -1208,16 +1208,16 @@
         </is>
       </c>
       <c r="B45">
-        <v>0.008160287291754666</v>
+        <v>0.008444545350068229</v>
       </c>
       <c r="C45">
-        <v>0.00750822112717872</v>
+        <v>0.0078077394021179</v>
       </c>
       <c r="D45">
-        <v>0.004415765717841744</v>
+        <v>0.004415765235740033</v>
       </c>
       <c r="E45">
-        <v>0.003973386880619191</v>
+        <v>0.003973386497893952</v>
       </c>
     </row>
     <row r="46">
@@ -1227,16 +1227,16 @@
         </is>
       </c>
       <c r="B46">
-        <v>0.01128362641883735</v>
+        <v>0.01284282613842817</v>
       </c>
       <c r="C46">
-        <v>0.01070740879093128</v>
+        <v>0.01232453445162514</v>
       </c>
       <c r="D46">
-        <v>0.003878039959123733</v>
+        <v>0.003878039754018153</v>
       </c>
       <c r="E46">
-        <v>0.003388304795514888</v>
+        <v>0.003388304516020685</v>
       </c>
     </row>
     <row r="47">
@@ -1246,16 +1246,16 @@
         </is>
       </c>
       <c r="B47">
-        <v>0.009317724502985609</v>
+        <v>0.008867060788130533</v>
       </c>
       <c r="C47">
-        <v>0.008771027170973458</v>
+        <v>0.008349659177591614</v>
       </c>
       <c r="D47">
-        <v>0.00488952137096842</v>
+        <v>0.004889522019708366</v>
       </c>
       <c r="E47">
-        <v>0.004538953336002602</v>
+        <v>0.004538953947857648</v>
       </c>
     </row>
     <row r="48">
@@ -1265,16 +1265,16 @@
         </is>
       </c>
       <c r="B48">
-        <v>0.006430828642833414</v>
+        <v>0.006782425357385952</v>
       </c>
       <c r="C48">
-        <v>0.005980793282484521</v>
+        <v>0.006327632261556487</v>
       </c>
       <c r="D48">
-        <v>0.003786344020771993</v>
+        <v>0.003786344130460266</v>
       </c>
       <c r="E48">
-        <v>0.003433140915458698</v>
+        <v>0.003433140993657311</v>
       </c>
     </row>
     <row r="49">
@@ -1284,16 +1284,16 @@
         </is>
       </c>
       <c r="B49">
-        <v>0.00567053136043168</v>
+        <v>0.005724955558346611</v>
       </c>
       <c r="C49">
-        <v>0.004937623791682348</v>
+        <v>0.004991171072506509</v>
       </c>
       <c r="D49">
-        <v>0.003272073411936395</v>
+        <v>0.003272074258322609</v>
       </c>
       <c r="E49">
-        <v>0.002775377249096812</v>
+        <v>0.002775378055738081</v>
       </c>
     </row>
     <row r="50">
@@ -1303,16 +1303,16 @@
         </is>
       </c>
       <c r="B50">
-        <v>0.01274123070633031</v>
+        <v>0.01300611078648318</v>
       </c>
       <c r="C50">
-        <v>0.01183698100930756</v>
+        <v>0.01215031236271061</v>
       </c>
       <c r="D50">
-        <v>0.008345517900613001</v>
+        <v>0.008345518488493978</v>
       </c>
       <c r="E50">
-        <v>0.007725213939243207</v>
+        <v>0.007725214602017109</v>
       </c>
     </row>
     <row r="51">
@@ -1322,16 +1322,16 @@
         </is>
       </c>
       <c r="B51">
-        <v>0.002031931757586814</v>
+        <v>0.002095486872443654</v>
       </c>
       <c r="C51">
-        <v>0.001433693255994244</v>
+        <v>0.001518646561773133</v>
       </c>
       <c r="D51">
-        <v>0.001363815388569738</v>
+        <v>0.001363816653739695</v>
       </c>
       <c r="E51">
-        <v>0.0009536728367573426</v>
+        <v>0.0009536741646104693</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ReadMes, Master, and drop what we do not need
This commit uploads a master .Rmd file to run all the Data codes scripts, it also includes a Read Me for raw data, and it drops the raw data files that we do not use.
</commit_message>
<xml_diff>
--- a/1-Data-Codes/2-Final_Data/exposures.xlsx
+++ b/1-Data-Codes/2-Final_Data/exposures.xlsx
@@ -391,10 +391,10 @@
         </is>
       </c>
       <c r="B2">
-        <v>0.01616742878187598</v>
+        <v>0.01920575862385186</v>
       </c>
       <c r="C2">
-        <v>0.01535950246713094</v>
+        <v>0.01839726259249032</v>
       </c>
       <c r="D2">
         <v>0.01040797675305219</v>
@@ -410,10 +410,10 @@
         </is>
       </c>
       <c r="B3">
-        <v>0.001114328573829887</v>
+        <v>0.001064138061892812</v>
       </c>
       <c r="C3">
-        <v>0.0008352419201105366</v>
+        <v>0.0008082525302238869</v>
       </c>
       <c r="D3">
         <v>0.00064097576404339</v>
@@ -429,10 +429,10 @@
         </is>
       </c>
       <c r="B4">
-        <v>0.009290194329385984</v>
+        <v>0.008852108084066361</v>
       </c>
       <c r="C4">
-        <v>0.008958292485214825</v>
+        <v>0.008503132250578369</v>
       </c>
       <c r="D4">
         <v>0.004893051700205482</v>
@@ -448,10 +448,10 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.01082461737011016</v>
+        <v>0.01162382832018563</v>
       </c>
       <c r="C5">
-        <v>0.01005121773483124</v>
+        <v>0.01079910249285568</v>
       </c>
       <c r="D5">
         <v>0.007844856199036571</v>
@@ -467,10 +467,10 @@
         </is>
       </c>
       <c r="B6">
-        <v>0.01319984283752404</v>
+        <v>0.01310785847144857</v>
       </c>
       <c r="C6">
-        <v>0.01277067466336601</v>
+        <v>0.0126777167528194</v>
       </c>
       <c r="D6">
         <v>0.007112328793891514</v>
@@ -486,10 +486,10 @@
         </is>
       </c>
       <c r="B7">
-        <v>0.008543329123849633</v>
+        <v>0.007996963228433698</v>
       </c>
       <c r="C7">
-        <v>0.008199587688978913</v>
+        <v>0.00765723651442295</v>
       </c>
       <c r="D7">
         <v>0.003724351013207759</v>
@@ -505,10 +505,10 @@
         </is>
       </c>
       <c r="B8">
-        <v>0.01046547667246475</v>
+        <v>0.01033656794316028</v>
       </c>
       <c r="C8">
-        <v>0.009978790217379128</v>
+        <v>0.009848681964819243</v>
       </c>
       <c r="D8">
         <v>0.006377560521764486</v>
@@ -524,10 +524,10 @@
         </is>
       </c>
       <c r="B9">
-        <v>0.006746097520709175</v>
+        <v>0.00655438950285438</v>
       </c>
       <c r="C9">
-        <v>0.006172798679333302</v>
+        <v>0.005986586714858723</v>
       </c>
       <c r="D9">
         <v>0.003954659092644731</v>
@@ -543,10 +543,10 @@
         </is>
       </c>
       <c r="B10">
-        <v>0.005483029921715594</v>
+        <v>0.005495316962924584</v>
       </c>
       <c r="C10">
-        <v>0.005155526931975511</v>
+        <v>0.00516523313532423</v>
       </c>
       <c r="D10">
         <v>0.003090602083261646</v>
@@ -562,10 +562,10 @@
         </is>
       </c>
       <c r="B11">
-        <v>0.01448594085095975</v>
+        <v>0.01546708864584439</v>
       </c>
       <c r="C11">
-        <v>0.01384006079669633</v>
+        <v>0.0147821056476489</v>
       </c>
       <c r="D11">
         <v>0.009090666601977554</v>
@@ -581,10 +581,10 @@
         </is>
       </c>
       <c r="B12">
-        <v>0.002000943134382114</v>
+        <v>0.001847830307249822</v>
       </c>
       <c r="C12">
-        <v>0.00183203518568754</v>
+        <v>0.001682566464049793</v>
       </c>
       <c r="D12">
         <v>0.001250260188395416</v>
@@ -600,10 +600,10 @@
         </is>
       </c>
       <c r="B13">
-        <v>0.01091110483096589</v>
+        <v>0.009199343067260305</v>
       </c>
       <c r="C13">
-        <v>0.01054835723117971</v>
+        <v>0.008800877749656317</v>
       </c>
       <c r="D13">
         <v>0.00544322307014899</v>
@@ -619,10 +619,10 @@
         </is>
       </c>
       <c r="B14">
-        <v>0.01076224225654533</v>
+        <v>0.01076903227993569</v>
       </c>
       <c r="C14">
-        <v>0.01016446463892172</v>
+        <v>0.01013568676445963</v>
       </c>
       <c r="D14">
         <v>0.006702984189505901</v>
@@ -638,10 +638,10 @@
         </is>
       </c>
       <c r="B15">
-        <v>0.01211972355305121</v>
+        <v>0.01277846220815438</v>
       </c>
       <c r="C15">
-        <v>0.01120085889924361</v>
+        <v>0.01179083810006734</v>
       </c>
       <c r="D15">
         <v>0.00842564417297337</v>
@@ -657,10 +657,10 @@
         </is>
       </c>
       <c r="B16">
-        <v>0.01136176617822109</v>
+        <v>0.01176830802169335</v>
       </c>
       <c r="C16">
-        <v>0.01071036825864781</v>
+        <v>0.01107051633922004</v>
       </c>
       <c r="D16">
         <v>0.005820276668568027</v>
@@ -676,10 +676,10 @@
         </is>
       </c>
       <c r="B17">
-        <v>0.006688846828023988</v>
+        <v>0.006642182627982343</v>
       </c>
       <c r="C17">
-        <v>0.006054300513150836</v>
+        <v>0.00599061023291184</v>
       </c>
       <c r="D17">
         <v>0.004180089349575281</v>
@@ -695,10 +695,10 @@
         </is>
       </c>
       <c r="B18">
-        <v>0.01129602691239412</v>
+        <v>0.0113937526231923</v>
       </c>
       <c r="C18">
-        <v>0.01052716486314972</v>
+        <v>0.01062422407590594</v>
       </c>
       <c r="D18">
         <v>0.007449106164755814</v>
@@ -714,10 +714,10 @@
         </is>
       </c>
       <c r="B19">
-        <v>0.004499584297299004</v>
+        <v>0.004652091949659546</v>
       </c>
       <c r="C19">
-        <v>0.003941025107596979</v>
+        <v>0.004074712925308041</v>
       </c>
       <c r="D19">
         <v>0.002718475176371824</v>
@@ -733,10 +733,10 @@
         </is>
       </c>
       <c r="B20">
-        <v>0.01084744266142097</v>
+        <v>0.01101265882153494</v>
       </c>
       <c r="C20">
-        <v>0.01030271913191642</v>
+        <v>0.01043836616177144</v>
       </c>
       <c r="D20">
         <v>0.006697436175344562</v>
@@ -752,10 +752,10 @@
         </is>
       </c>
       <c r="B21">
-        <v>0.005576508910145192</v>
+        <v>0.005720049786656569</v>
       </c>
       <c r="C21">
-        <v>0.005295299990651683</v>
+        <v>0.005426612069355069</v>
       </c>
       <c r="D21">
         <v>0.002801671083293092</v>
@@ -771,10 +771,10 @@
         </is>
       </c>
       <c r="B22">
-        <v>0.01325244862305611</v>
+        <v>0.0131592422691012</v>
       </c>
       <c r="C22">
-        <v>0.01284031242119282</v>
+        <v>0.01272897061110782</v>
       </c>
       <c r="D22">
         <v>0.00713227731343879</v>
@@ -790,10 +790,10 @@
         </is>
       </c>
       <c r="B23">
-        <v>0.009144640966304907</v>
+        <v>0.009301068056193877</v>
       </c>
       <c r="C23">
-        <v>0.008311652321969835</v>
+        <v>0.00845082879195899</v>
       </c>
       <c r="D23">
         <v>0.007163586037232712</v>
@@ -809,10 +809,10 @@
         </is>
       </c>
       <c r="B24">
-        <v>0.01119555474451042</v>
+        <v>0.01092093823701653</v>
       </c>
       <c r="C24">
-        <v>0.01056478702123411</v>
+        <v>0.01025866467831401</v>
       </c>
       <c r="D24">
         <v>0.006256189675348401</v>
@@ -828,10 +828,10 @@
         </is>
       </c>
       <c r="B25">
-        <v>0.0126824240012623</v>
+        <v>0.01413927579208907</v>
       </c>
       <c r="C25">
-        <v>0.01176528219418757</v>
+        <v>0.01312666093257296</v>
       </c>
       <c r="D25">
         <v>0.009116557752357634</v>
@@ -847,10 +847,10 @@
         </is>
       </c>
       <c r="B26">
-        <v>0.009095738901378608</v>
+        <v>0.009815293322239032</v>
       </c>
       <c r="C26">
-        <v>0.008479899085518381</v>
+        <v>0.009154219549078035</v>
       </c>
       <c r="D26">
         <v>0.005403753804922695</v>
@@ -866,10 +866,10 @@
         </is>
       </c>
       <c r="B27">
-        <v>0.002886496802688513</v>
+        <v>0.002692378212257929</v>
       </c>
       <c r="C27">
-        <v>0.002551242442908614</v>
+        <v>0.002344968518395085</v>
       </c>
       <c r="D27">
         <v>0.001546523188141996</v>
@@ -885,10 +885,10 @@
         </is>
       </c>
       <c r="B28">
-        <v>0.007688735113494544</v>
+        <v>0.007476652159740717</v>
       </c>
       <c r="C28">
-        <v>0.007178040746313545</v>
+        <v>0.006961431751116719</v>
       </c>
       <c r="D28">
         <v>0.004541879024141163</v>
@@ -904,10 +904,10 @@
         </is>
       </c>
       <c r="B29">
-        <v>0.003102805861250911</v>
+        <v>0.003060806751247731</v>
       </c>
       <c r="C29">
-        <v>0.002783625130653979</v>
+        <v>0.002722908264783516</v>
       </c>
       <c r="D29">
         <v>0.001671506828818534</v>
@@ -923,10 +923,10 @@
         </is>
       </c>
       <c r="B30">
-        <v>0.01881836802423357</v>
+        <v>0.01690982566731769</v>
       </c>
       <c r="C30">
-        <v>0.01831705023945007</v>
+        <v>0.01635913006396045</v>
       </c>
       <c r="D30">
         <v>0.01008627771016791</v>
@@ -942,10 +942,10 @@
         </is>
       </c>
       <c r="B31">
-        <v>0.009520582340971785</v>
+        <v>0.009468426512062022</v>
       </c>
       <c r="C31">
-        <v>0.009021481541213466</v>
+        <v>0.008960878809554346</v>
       </c>
       <c r="D31">
         <v>0.005017335486240285</v>
@@ -961,10 +961,10 @@
         </is>
       </c>
       <c r="B32">
-        <v>0.005710218460705146</v>
+        <v>0.005270645194737429</v>
       </c>
       <c r="C32">
-        <v>0.005363264944307802</v>
+        <v>0.004906702433299757</v>
       </c>
       <c r="D32">
         <v>0.003088792580914898</v>
@@ -980,10 +980,10 @@
         </is>
       </c>
       <c r="B33">
-        <v>0.009059947259411177</v>
+        <v>0.009263276794848814</v>
       </c>
       <c r="C33">
-        <v>0.008633744800545042</v>
+        <v>0.008796666386126834</v>
       </c>
       <c r="D33">
         <v>0.005452604803692462</v>
@@ -999,10 +999,10 @@
         </is>
       </c>
       <c r="B34">
-        <v>0.02147791671006524</v>
+        <v>0.02216435593903705</v>
       </c>
       <c r="C34">
-        <v>0.02053408070452858</v>
+        <v>0.02119656461300347</v>
       </c>
       <c r="D34">
         <v>0.01383363520534461</v>
@@ -1018,10 +1018,10 @@
         </is>
       </c>
       <c r="B35">
-        <v>0.004288885526765049</v>
+        <v>0.003990259541291106</v>
       </c>
       <c r="C35">
-        <v>0.003923283735257924</v>
+        <v>0.00362968705967037</v>
       </c>
       <c r="D35">
         <v>0.002309732435280013</v>
@@ -1037,10 +1037,10 @@
         </is>
       </c>
       <c r="B36">
-        <v>0.01121122143878064</v>
+        <v>0.01158216091667626</v>
       </c>
       <c r="C36">
-        <v>0.01034648976974103</v>
+        <v>0.01066680234055278</v>
       </c>
       <c r="D36">
         <v>0.007246972246919058</v>
@@ -1056,10 +1056,10 @@
         </is>
       </c>
       <c r="B37">
-        <v>0.007799390664922923</v>
+        <v>0.008123718473361137</v>
       </c>
       <c r="C37">
-        <v>0.007153638715240352</v>
+        <v>0.007430775916479243</v>
       </c>
       <c r="D37">
         <v>0.00453489937991951</v>
@@ -1075,10 +1075,10 @@
         </is>
       </c>
       <c r="B38">
-        <v>0.0113117412255217</v>
+        <v>0.01056937582347497</v>
       </c>
       <c r="C38">
-        <v>0.0108809700301654</v>
+        <v>0.01012769542607296</v>
       </c>
       <c r="D38">
         <v>0.00610976309272813</v>
@@ -1094,10 +1094,10 @@
         </is>
       </c>
       <c r="B39">
-        <v>0.01145575416434506</v>
+        <v>0.01214691883466968</v>
       </c>
       <c r="C39">
-        <v>0.01074719872271248</v>
+        <v>0.01136663061839803</v>
       </c>
       <c r="D39">
         <v>0.007340469606039235</v>
@@ -1113,10 +1113,10 @@
         </is>
       </c>
       <c r="B40">
-        <v>0.0150075520340855</v>
+        <v>0.01501295460503677</v>
       </c>
       <c r="C40">
-        <v>0.01421536947059665</v>
+        <v>0.01423001103437266</v>
       </c>
       <c r="D40">
         <v>0.008319534145116261</v>
@@ -1132,10 +1132,10 @@
         </is>
       </c>
       <c r="B41">
-        <v>0.02068201334671391</v>
+        <v>0.02186737697738161</v>
       </c>
       <c r="C41">
-        <v>0.0198143654646785</v>
+        <v>0.02095774614015161</v>
       </c>
       <c r="D41">
         <v>0.01333165186640678</v>
@@ -1151,10 +1151,10 @@
         </is>
       </c>
       <c r="B42">
-        <v>0.008408932922103374</v>
+        <v>0.007533601744883829</v>
       </c>
       <c r="C42">
-        <v>0.007914856691945908</v>
+        <v>0.007068762379145454</v>
       </c>
       <c r="D42">
         <v>0.005118709533145206</v>
@@ -1170,10 +1170,10 @@
         </is>
       </c>
       <c r="B43">
-        <v>0.01349271310064208</v>
+        <v>0.01451043534403035</v>
       </c>
       <c r="C43">
-        <v>0.01266955291028146</v>
+        <v>0.01363491576123427</v>
       </c>
       <c r="D43">
         <v>0.008366784789245758</v>
@@ -1189,10 +1189,10 @@
         </is>
       </c>
       <c r="B44">
-        <v>0.009571082311229008</v>
+        <v>0.009210328532476136</v>
       </c>
       <c r="C44">
-        <v>0.009073167220271241</v>
+        <v>0.008688224193069305</v>
       </c>
       <c r="D44">
         <v>0.005161834156403239</v>
@@ -1208,10 +1208,10 @@
         </is>
       </c>
       <c r="B45">
-        <v>0.008444545350068229</v>
+        <v>0.008160287291754664</v>
       </c>
       <c r="C45">
-        <v>0.0078077394021179</v>
+        <v>0.007508221127178719</v>
       </c>
       <c r="D45">
         <v>0.004415765235740033</v>
@@ -1227,10 +1227,10 @@
         </is>
       </c>
       <c r="B46">
-        <v>0.01284282613842817</v>
+        <v>0.01128362641883733</v>
       </c>
       <c r="C46">
-        <v>0.01232453445162514</v>
+        <v>0.01070740879093126</v>
       </c>
       <c r="D46">
         <v>0.003878039754018153</v>
@@ -1246,10 +1246,10 @@
         </is>
       </c>
       <c r="B47">
-        <v>0.008867060788130533</v>
+        <v>0.009317724502985613</v>
       </c>
       <c r="C47">
-        <v>0.008349659177591614</v>
+        <v>0.00877102717097346</v>
       </c>
       <c r="D47">
         <v>0.004889522019708366</v>
@@ -1265,10 +1265,10 @@
         </is>
       </c>
       <c r="B48">
-        <v>0.006782425357385952</v>
+        <v>0.006430828642833402</v>
       </c>
       <c r="C48">
-        <v>0.006327632261556487</v>
+        <v>0.00598079328248451</v>
       </c>
       <c r="D48">
         <v>0.003786344130460266</v>
@@ -1284,10 +1284,10 @@
         </is>
       </c>
       <c r="B49">
-        <v>0.005724955558346611</v>
+        <v>0.005670531360431683</v>
       </c>
       <c r="C49">
-        <v>0.004991171072506509</v>
+        <v>0.004937623791682351</v>
       </c>
       <c r="D49">
         <v>0.003272074258322609</v>
@@ -1303,10 +1303,10 @@
         </is>
       </c>
       <c r="B50">
-        <v>0.01300611078648318</v>
+        <v>0.01274123070633032</v>
       </c>
       <c r="C50">
-        <v>0.01215031236271061</v>
+        <v>0.01183698100930756</v>
       </c>
       <c r="D50">
         <v>0.008345518488493978</v>
@@ -1322,10 +1322,10 @@
         </is>
       </c>
       <c r="B51">
-        <v>0.002095486872443654</v>
+        <v>0.002031931757586819</v>
       </c>
       <c r="C51">
-        <v>0.001518646561773133</v>
+        <v>0.001433693255994247</v>
       </c>
       <c r="D51">
         <v>0.001363816653739695</v>

</xml_diff>